<commit_message>
Add theoretical maximum array sizes for 10 minutes
</commit_message>
<xml_diff>
--- a/runtime_analysis.xlsx
+++ b/runtime_analysis.xlsx
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
   <si>
     <t>Runtimes for maximum sub-array algorithms (seconds)</t>
   </si>
@@ -78,6 +78,9 @@
   </si>
   <si>
     <t>R^2 for Alg 3, nlgn:</t>
+  </si>
+  <si>
+    <t>Theoretical maximum array size that can be solved in ten minutes</t>
   </si>
 </sst>
 </file>
@@ -112,7 +115,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -130,7 +133,9 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top style="medium">
         <color indexed="64"/>
@@ -141,8 +146,72 @@
     <border>
       <left/>
       <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
       <top/>
       <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -330,9 +399,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -341,62 +410,88 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2637,8 +2732,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:M14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="S18" sqref="S18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2651,6 +2746,10 @@
     <col min="6" max="6" width="14.28515625" customWidth="1"/>
     <col min="7" max="7" width="17.42578125" customWidth="1"/>
     <col min="8" max="8" width="25.140625" customWidth="1"/>
+    <col min="10" max="10" width="16.85546875" customWidth="1"/>
+    <col min="11" max="11" width="17" customWidth="1"/>
+    <col min="12" max="12" width="15.7109375" customWidth="1"/>
+    <col min="13" max="13" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2666,24 +2765,38 @@
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="21"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="20"/>
+      <c r="J2" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" s="27"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="28"/>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B3" s="5"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="22"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="21"/>
+      <c r="J3" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="K3" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="L3" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="M3" s="30" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="6" t="s">
         <v>5</v>
       </c>
@@ -2696,35 +2809,47 @@
       <c r="E4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="15" t="s">
+      <c r="G4" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="22"/>
+      <c r="H4" s="21"/>
+      <c r="J4" s="31">
+        <v>3533</v>
+      </c>
+      <c r="K4" s="32">
+        <v>127526</v>
+      </c>
+      <c r="L4" s="32">
+        <v>48170800</v>
+      </c>
+      <c r="M4" s="33">
+        <v>1999999933</v>
+      </c>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B5" s="5">
         <v>10</v>
       </c>
-      <c r="C5" s="16">
+      <c r="C5" s="15">
         <v>1.4615058898899999E-4</v>
       </c>
-      <c r="D5" s="16">
+      <c r="D5" s="15">
         <v>5.1975250244100001E-5</v>
       </c>
-      <c r="E5" s="16">
+      <c r="E5" s="15">
         <v>8.1062316894499998E-5</v>
       </c>
-      <c r="F5" s="17">
+      <c r="F5" s="16">
         <v>1.5974044799799998E-5</v>
       </c>
-      <c r="G5" s="18">
+      <c r="G5" s="17">
         <f>B5 * LOG(B5, 2) * $H$9</f>
         <v>1.6212463378899999E-5</v>
       </c>
-      <c r="H5" s="23" t="s">
+      <c r="H5" s="22" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2732,23 +2857,23 @@
       <c r="B6" s="5">
         <v>20</v>
       </c>
-      <c r="C6" s="16">
+      <c r="C6" s="15">
         <v>6.7710876464800002E-4</v>
       </c>
-      <c r="D6" s="16">
+      <c r="D6" s="15">
         <v>1.5497207641600001E-4</v>
       </c>
-      <c r="E6" s="16">
+      <c r="E6" s="15">
         <v>1.52111053467E-4</v>
       </c>
-      <c r="F6" s="17">
+      <c r="F6" s="16">
         <v>2.3126602172899999E-5</v>
       </c>
-      <c r="G6" s="18">
+      <c r="G6" s="17">
         <f>B6 * LOG(B6, 2) * $H$9</f>
         <v>4.2185802319105437E-5</v>
       </c>
-      <c r="H6" s="22">
+      <c r="H6" s="21">
         <f>RSQ(E5:E14, G5:G14)</f>
         <v>0.99861016739292163</v>
       </c>
@@ -2757,45 +2882,45 @@
       <c r="B7" s="5">
         <v>40</v>
       </c>
-      <c r="C7" s="16">
+      <c r="C7" s="15">
         <v>3.8380622863800002E-3</v>
       </c>
-      <c r="D7" s="16">
+      <c r="D7" s="15">
         <v>4.9901008605999998E-4</v>
       </c>
-      <c r="E7" s="16">
+      <c r="E7" s="15">
         <v>3.1280517578099998E-4</v>
       </c>
-      <c r="F7" s="17">
+      <c r="F7" s="16">
         <v>3.5047531127900001E-5</v>
       </c>
-      <c r="G7" s="18">
+      <c r="G7" s="17">
         <f>B7 * LOG(B7, 2) * $H$9</f>
         <v>1.0389335576082177E-4</v>
       </c>
-      <c r="H7" s="22"/>
+      <c r="H7" s="21"/>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B8" s="5">
         <v>80</v>
       </c>
-      <c r="C8" s="16">
+      <c r="C8" s="15">
         <v>2.4200916290299999E-2</v>
       </c>
-      <c r="D8" s="16">
+      <c r="D8" s="15">
         <v>1.8320083618199999E-3</v>
       </c>
-      <c r="E8" s="16">
+      <c r="E8" s="15">
         <v>6.4516067504899997E-4</v>
       </c>
-      <c r="F8" s="17">
+      <c r="F8" s="16">
         <v>6.2942504882800005E-5</v>
       </c>
-      <c r="G8" s="18">
+      <c r="G8" s="17">
         <f t="shared" ref="G6:G14" si="0">B8 * LOG(B8, 2) * $H$9</f>
         <v>2.4683021376686529E-4</v>
       </c>
-      <c r="H8" s="22" t="s">
+      <c r="H8" s="21" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2803,23 +2928,23 @@
       <c r="B9" s="5">
         <v>160</v>
       </c>
-      <c r="C9" s="16">
+      <c r="C9" s="15">
         <v>0.16966009139999999</v>
       </c>
-      <c r="D9" s="16">
+      <c r="D9" s="15">
         <v>7.0810317993199997E-3</v>
       </c>
-      <c r="E9" s="16">
+      <c r="E9" s="15">
         <v>1.36494636536E-3</v>
       </c>
-      <c r="F9" s="17">
+      <c r="F9" s="16">
         <v>1.16109848022E-4</v>
       </c>
-      <c r="G9" s="18">
+      <c r="G9" s="17">
         <f t="shared" si="0"/>
         <v>5.7174743202417408E-4</v>
       </c>
-      <c r="H9" s="22">
+      <c r="H9" s="21">
         <f xml:space="preserve"> ($E$5 / ($B$5 * LOG($B$5, 2) * 5) )</f>
         <v>4.8804377806527206E-7</v>
       </c>
@@ -2828,115 +2953,116 @@
       <c r="B10" s="5">
         <v>320</v>
       </c>
-      <c r="C10" s="16">
+      <c r="C10" s="15">
         <v>0.80736088752699997</v>
       </c>
-      <c r="D10" s="16">
+      <c r="D10" s="15">
         <v>1.19590759277E-2</v>
       </c>
-      <c r="E10" s="16">
+      <c r="E10" s="15">
         <v>1.1248588562000001E-3</v>
       </c>
-      <c r="F10" s="17">
+      <c r="F10" s="16">
         <v>8.5115432739300002E-5</v>
       </c>
-      <c r="G10" s="18">
+      <c r="G10" s="17">
         <f t="shared" si="0"/>
         <v>1.2996688730292352E-3</v>
       </c>
-      <c r="H10" s="22"/>
+      <c r="H10" s="21"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B11" s="5">
         <v>640</v>
       </c>
-      <c r="C11" s="16">
+      <c r="C11" s="15">
         <v>3.8955600261700001</v>
       </c>
-      <c r="D11" s="16">
+      <c r="D11" s="15">
         <v>4.7562122344999999E-2</v>
       </c>
-      <c r="E11" s="16">
+      <c r="E11" s="15">
         <v>2.3748874664300001E-3</v>
       </c>
-      <c r="F11" s="17">
+      <c r="F11" s="16">
         <v>1.6498565673800001E-4</v>
       </c>
-      <c r="G11" s="18">
+      <c r="G11" s="17">
         <f>B11 * LOG(B11, 2) * $H$9</f>
         <v>2.9116857640202444E-3</v>
       </c>
-      <c r="H11" s="22"/>
+      <c r="H11" s="21"/>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B12" s="5">
         <v>1280</v>
       </c>
-      <c r="C12" s="16">
+      <c r="C12" s="15">
         <v>31.423593998000001</v>
       </c>
-      <c r="D12" s="16">
+      <c r="D12" s="15">
         <v>0.19263505935700001</v>
       </c>
-      <c r="E12" s="16">
+      <c r="E12" s="15">
         <v>5.0539970397899996E-3</v>
       </c>
-      <c r="F12" s="17">
+      <c r="F12" s="16">
         <v>3.2997131347699998E-4</v>
       </c>
-      <c r="G12" s="18">
+      <c r="G12" s="17">
         <f t="shared" si="0"/>
         <v>6.448067563964037E-3</v>
       </c>
-      <c r="H12" s="22"/>
+      <c r="H12" s="21"/>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B13" s="5">
         <v>2560</v>
       </c>
-      <c r="C13" s="16">
+      <c r="C13" s="15">
         <v>253.22493696199999</v>
       </c>
-      <c r="D13" s="16">
+      <c r="D13" s="15">
         <v>0.77345800399800002</v>
       </c>
-      <c r="E13" s="16">
+      <c r="E13" s="15">
         <v>1.05469226837E-2</v>
       </c>
-      <c r="F13" s="17">
+      <c r="F13" s="16">
         <v>6.5493583679199999E-4</v>
       </c>
-      <c r="G13" s="18">
+      <c r="G13" s="17">
         <f t="shared" si="0"/>
         <v>1.4145527199775172E-2</v>
       </c>
-      <c r="H13" s="22"/>
+      <c r="H13" s="21"/>
     </row>
     <row r="14" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="7">
         <v>5120</v>
       </c>
-      <c r="C14" s="19">
+      <c r="C14" s="18">
         <v>2055.3600599800002</v>
       </c>
-      <c r="D14" s="19">
+      <c r="D14" s="18">
         <v>3.1561529636399999</v>
       </c>
-      <c r="E14" s="19">
+      <c r="E14" s="18">
         <v>2.2043943405199998E-2</v>
       </c>
-      <c r="F14" s="20">
+      <c r="F14" s="19">
         <v>1.3351440429700001E-3</v>
       </c>
-      <c r="G14" s="25">
+      <c r="G14" s="24">
         <f t="shared" si="0"/>
         <v>3.0789838543244536E-2</v>
       </c>
-      <c r="H14" s="24"/>
+      <c r="H14" s="23"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="C2:F2"/>
+    <mergeCell ref="J2:M2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>